<commit_message>
Seed change + starting to import PPO
</commit_message>
<xml_diff>
--- a/resultat_DPO_summarization.xlsx
+++ b/resultat_DPO_summarization.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="57">
   <si>
     <t>Model</t>
   </si>
   <si>
+    <t>Beta</t>
+  </si>
+  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -34,6 +37,9 @@
     <t>DPO</t>
   </si>
   <si>
+    <t>0.1</t>
+  </si>
+  <si>
     <t>0.25</t>
   </si>
   <si>
@@ -52,21 +58,21 @@
     <t>0.75</t>
   </si>
   <si>
+    <t>48 min</t>
+  </si>
+  <si>
     <t>1.0331</t>
   </si>
   <si>
-    <t>48 min</t>
-  </si>
-  <si>
     <t>0.540</t>
   </si>
   <si>
+    <t>58 min</t>
+  </si>
+  <si>
     <t>1.0280</t>
   </si>
   <si>
-    <t>58 min</t>
-  </si>
-  <si>
     <t>0.400</t>
   </si>
   <si>
@@ -79,9 +85,6 @@
     <t>SFT</t>
   </si>
   <si>
-    <t>0.1</t>
-  </si>
-  <si>
     <t>0.520</t>
   </si>
   <si>
@@ -140,6 +143,45 @@
   </si>
   <si>
     <t>2000train/100test/maxtoken64</t>
+  </si>
+  <si>
+    <t>0.560</t>
+  </si>
+  <si>
+    <t>0.0176</t>
+  </si>
+  <si>
+    <t>trop proche</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>1.1725</t>
+  </si>
+  <si>
+    <t>0.570</t>
+  </si>
+  <si>
+    <t>1.1685</t>
+  </si>
+  <si>
+    <t>0.670</t>
+  </si>
+  <si>
+    <t>1.1735</t>
+  </si>
+  <si>
+    <t>1.1676</t>
+  </si>
+  <si>
+    <t>0.450</t>
+  </si>
+  <si>
+    <t>0.290</t>
+  </si>
+  <si>
+    <t>0.630</t>
   </si>
 </sst>
 </file>
@@ -149,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m.yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -176,6 +218,11 @@
       <color rgb="FF1F1F1F"/>
       <name val="Monospace"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -197,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -207,7 +254,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -216,10 +269,20 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -440,6 +503,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="7" max="7" width="20.38"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -460,163 +526,228 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
         <v>55.0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
         <v>1.0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2">
         <v>57.0</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
+      <c r="E4" s="3">
+        <v>1.0331</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.028</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -624,116 +755,358 @@
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
+      <c r="E14" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
         <v>1.0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
+      <c r="E16" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>25</v>
+      <c r="E17" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="7">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1.6287</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="12">
         <v>1602321.0</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1638115.0</v>
-      </c>
-      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="E19" s="13">
+        <v>1.6385</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1638115.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
         <v>1.0</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1.1725</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1.1685</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.1767</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1.1751</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.1632</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.1862</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.1745</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.1803</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.1802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>